<commit_message>
#mod. en camote y utils.R
</commit_message>
<xml_diff>
--- a/camote.xlsx
+++ b/camote.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OMAR_2016\R_UNALM\cropdatape\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
@@ -2500,9 +2505,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t>sowva</t>
-  </si>
-  <si>
     <t>harva</t>
   </si>
   <si>
@@ -2512,13 +2514,16 @@
     <t>ayield</t>
   </si>
   <si>
-    <t>applot</t>
+    <t>pricePlot</t>
+  </si>
+  <si>
+    <t>sowa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2566,6 +2571,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2852,15 +2860,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4234,7 +4245,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -5603,7 +5614,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -6972,7 +6983,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -8341,7 +8352,7 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>